<commit_message>
last update (safe backup)
</commit_message>
<xml_diff>
--- a/Model2/excel/DemR/results/Overview_fullweek_DR.xlsx
+++ b/Model2/excel/DemR/results/Overview_fullweek_DR.xlsx
@@ -7,16 +7,166 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="reserves" sheetId="1" r:id="rId1"/>
+    <sheet name="capacities" sheetId="2" r:id="rId2"/>
+    <sheet name="storage" sheetId="3" r:id="rId3"/>
+    <sheet name="generation" sheetId="4" r:id="rId4"/>
+    <sheet name="demandshift" sheetId="5" r:id="rId5"/>
+    <sheet name="curtailment" sheetId="6" r:id="rId6"/>
+    <sheet name="storc" sheetId="7" r:id="rId7"/>
+    <sheet name="stordisc" sheetId="8" r:id="rId8"/>
+    <sheet name="maxshift" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="43">
+  <si>
+    <t>generation</t>
+  </si>
+  <si>
+    <t>storage</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t>generation30</t>
+  </si>
+  <si>
+    <t>storage30</t>
+  </si>
+  <si>
+    <t>DR30</t>
+  </si>
+  <si>
+    <t>generation50</t>
+  </si>
+  <si>
+    <t>storage50</t>
+  </si>
+  <si>
+    <t>DR50</t>
+  </si>
+  <si>
+    <t>generation70</t>
+  </si>
+  <si>
+    <t>storage70</t>
+  </si>
+  <si>
+    <t>DR70</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>AFRR_DN</t>
+  </si>
+  <si>
+    <t>AFRR_UP</t>
+  </si>
+  <si>
+    <t>FCR_UP</t>
+  </si>
+  <si>
+    <t>MFRR_DN</t>
+  </si>
+  <si>
+    <t>MFRR_UP</t>
+  </si>
+  <si>
+    <t>BEL</t>
+  </si>
+  <si>
+    <t>BEL30</t>
+  </si>
+  <si>
+    <t>BEL50</t>
+  </si>
+  <si>
+    <t>BEL70</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>BEL_Z</t>
+  </si>
+  <si>
+    <t>CCGT</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Nuclear</t>
+  </si>
+  <si>
+    <t>OCGT</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>WIND_OFF</t>
+  </si>
+  <si>
+    <t>WIND_ON</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>STOR_L</t>
+  </si>
+  <si>
+    <t>STOR_M_C</t>
+  </si>
+  <si>
+    <t>STOR_M_E</t>
+  </si>
+  <si>
+    <t>STOR_S</t>
+  </si>
+  <si>
+    <t>curt</t>
+  </si>
+  <si>
+    <t>curt30</t>
+  </si>
+  <si>
+    <t>curt50</t>
+  </si>
+  <si>
+    <t>curt70</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -32,7 +182,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +190,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,12 +508,1129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>1614553.22059607</v>
+      </c>
+      <c r="D2">
+        <v>35.5395867861186</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>2073491.71869695</v>
+      </c>
+      <c r="G2">
+        <v>566003.077220997</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1912492.64002023</v>
+      </c>
+      <c r="J2">
+        <v>1903726.68810267</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>2263267.45525479</v>
+      </c>
+      <c r="M2">
+        <v>1892672.88322897</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>285847.841700509</v>
+      </c>
+      <c r="D3">
+        <v>1354447.1318561</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>622385.326596478</v>
+      </c>
+      <c r="G3">
+        <v>2042778.7069809</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>891437.812536672</v>
+      </c>
+      <c r="J3">
+        <v>2950333.57641644</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>411701.381953746</v>
+      </c>
+      <c r="M3">
+        <v>3892350.9534278</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>27556.0023121239</v>
+      </c>
+      <c r="D4">
+        <v>848446.397687951</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>108651.249765019</v>
+      </c>
+      <c r="G4">
+        <v>767351.150234977</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>202817.822448209</v>
+      </c>
+      <c r="J4">
+        <v>673184.577551796</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>57912.6094467839</v>
+      </c>
+      <c r="M4">
+        <v>818089.790553237</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>9572929.73112173</v>
+      </c>
+      <c r="D5">
+        <v>904.330124281105</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>9970676.84345968</v>
+      </c>
+      <c r="G5">
+        <v>2995970.36317092</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>7913519.1054736</v>
+      </c>
+      <c r="J5">
+        <v>8948515.89492063</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>8339939.06785798</v>
+      </c>
+      <c r="M5">
+        <v>9644733.58618847</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>4625228.05011725</v>
+      </c>
+      <c r="D6">
+        <v>5194830.986412</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>5959628.88706362</v>
+      </c>
+      <c r="G6">
+        <v>7304253.30358973</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>4501248.31260845</v>
+      </c>
+      <c r="J6">
+        <v>12711597.9577207</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>2884237.36143534</v>
+      </c>
+      <c r="M6">
+        <v>16514749.1547212</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>3058.09922493337</v>
+      </c>
+      <c r="E2">
+        <v>4690.52947927332</v>
+      </c>
+      <c r="F2">
+        <v>8575.09279117594</v>
+      </c>
+      <c r="G2">
+        <v>5364.30872218796</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>1978.47731952343</v>
+      </c>
+      <c r="E3">
+        <v>1402.23913449796</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1675.04909691227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4">
+        <v>6883.27262901597</v>
+      </c>
+      <c r="E4">
+        <v>4251.3378459573</v>
+      </c>
+      <c r="F4">
+        <v>404.681898954117</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>838.998528549944</v>
+      </c>
+      <c r="E5">
+        <v>1098.43100751703</v>
+      </c>
+      <c r="F5">
+        <v>1449.46215392542</v>
+      </c>
+      <c r="G5">
+        <v>2495.16719278249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>3000</v>
+      </c>
+      <c r="E6">
+        <v>3000</v>
+      </c>
+      <c r="F6">
+        <v>3000</v>
+      </c>
+      <c r="G6">
+        <v>17235.9670006382</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>4606.96669095824</v>
+      </c>
+      <c r="E8">
+        <v>13117.8084415048</v>
+      </c>
+      <c r="F8">
+        <v>23389.496377585</v>
+      </c>
+      <c r="G8">
+        <v>27060.7435632053</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <v>1000</v>
+      </c>
+      <c r="F3">
+        <v>1000</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>580.308979228316</v>
+      </c>
+      <c r="E4">
+        <v>521.786515050647</v>
+      </c>
+      <c r="F4">
+        <v>4155.01021692498</v>
+      </c>
+      <c r="G4">
+        <v>6459.3498263973</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5">
+        <v>99.7331486797888</v>
+      </c>
+      <c r="E5">
+        <v>99.54772430012</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>99.9999999999991</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>12488319.348234</v>
+      </c>
+      <c r="D2">
+        <v>22626760.3815926</v>
+      </c>
+      <c r="E2">
+        <v>47233029.0501997</v>
+      </c>
+      <c r="F2">
+        <v>21159825.2761633</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>16002416.0331107</v>
+      </c>
+      <c r="D3">
+        <v>11157956.218542</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>11362587.5822128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>60293767.3040463</v>
+      </c>
+      <c r="D4">
+        <v>36935155.6095801</v>
+      </c>
+      <c r="E4">
+        <v>3369757.40758097</v>
+      </c>
+      <c r="F4">
+        <v>-1.40204580407032e-06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>612326.458236931</v>
+      </c>
+      <c r="D5">
+        <v>872907.239576282</v>
+      </c>
+      <c r="E5">
+        <v>813407.806952614</v>
+      </c>
+      <c r="F5">
+        <v>1407875.40099213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>3064318.49854914</v>
+      </c>
+      <c r="D6">
+        <v>3063472.28491221</v>
+      </c>
+      <c r="E6">
+        <v>3059069.57984012</v>
+      </c>
+      <c r="F6">
+        <v>17600373.7588503</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>9782849.56179962</v>
+      </c>
+      <c r="D8">
+        <v>27579712.9821679</v>
+      </c>
+      <c r="E8">
+        <v>48012811.2886143</v>
+      </c>
+      <c r="F8">
+        <v>53901561.4603696</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>4162211.25247893</v>
+      </c>
+      <c r="C2">
+        <v>5789309.67680081</v>
+      </c>
+      <c r="D2">
+        <v>8425723.20372216</v>
+      </c>
+      <c r="E2">
+        <v>8614404.66056837</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>276673.584217995</v>
+      </c>
+      <c r="D2">
+        <v>1659808.75245572</v>
+      </c>
+      <c r="E2">
+        <v>3566791.58092535</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B2">
+        <v>412253.443570518</v>
+      </c>
+      <c r="C2">
+        <v>383734.800186083</v>
+      </c>
+      <c r="D2">
+        <v>1396996.78421986</v>
+      </c>
+      <c r="E2">
+        <v>13231848.5974958</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>2050</v>
+      </c>
+      <c r="B2">
+        <v>312963.551131526</v>
+      </c>
+      <c r="C2">
+        <v>291720.974111042</v>
+      </c>
+      <c r="D2">
+        <v>1052683.38794821</v>
+      </c>
+      <c r="E2">
+        <v>9945246.86064202</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2224.15951619049</v>
+      </c>
+      <c r="C2">
+        <v>4852.95768558309</v>
+      </c>
+      <c r="D2">
+        <v>4889.57276278364</v>
+      </c>
+      <c r="E2">
+        <v>4889.57276278365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2312.8959089581</v>
+      </c>
+      <c r="C3">
+        <v>2321.30935452233</v>
+      </c>
+      <c r="D3">
+        <v>2321.30935452233</v>
+      </c>
+      <c r="E3">
+        <v>2321.30935452233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2312.8959089581</v>
+      </c>
+      <c r="C4">
+        <v>2321.30935452233</v>
+      </c>
+      <c r="D4">
+        <v>2321.30935452233</v>
+      </c>
+      <c r="E4">
+        <v>2321.30935452233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1454.5951456003</v>
+      </c>
+      <c r="C5">
+        <v>1454.5951456003</v>
+      </c>
+      <c r="D5">
+        <v>1454.5951456003</v>
+      </c>
+      <c r="E5">
+        <v>1454.5951456003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1454.5951456003</v>
+      </c>
+      <c r="C6">
+        <v>1454.5951456003</v>
+      </c>
+      <c r="D6">
+        <v>1454.5951456003</v>
+      </c>
+      <c r="E6">
+        <v>1454.5951456003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3610.51917214959</v>
+      </c>
+      <c r="C7">
+        <v>3610.51917214959</v>
+      </c>
+      <c r="D7">
+        <v>3596.11976307164</v>
+      </c>
+      <c r="E7">
+        <v>3610.51917214959</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3395.86819601824</v>
+      </c>
+      <c r="C8">
+        <v>3501.58090213772</v>
+      </c>
+      <c r="D8">
+        <v>3610.51917214959</v>
+      </c>
+      <c r="E8">
+        <v>3610.51917214959</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2947.07533505669</v>
+      </c>
+      <c r="C9">
+        <v>4857.62891670642</v>
+      </c>
+      <c r="D9">
+        <v>4857.62891670642</v>
+      </c>
+      <c r="E9">
+        <v>4857.62891670642</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>